<commit_message>
Updating wordpress table formatting - tests
</commit_message>
<xml_diff>
--- a/Gimp Maptile Plugin/Locations/FreeCityLandmarks.xlsx
+++ b/Gimp Maptile Plugin/Locations/FreeCityLandmarks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amele\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Development\Workspace\Merisyl\Gimp Maptile Plugin\Locations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1CF93B-9FE2-4A9D-9B9C-72DCE88BA660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F899F6F-7136-47DC-A1D2-F033B3F2DD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{86C0CD85-1229-4AB4-A667-7C169E5D8340}"/>
   </bookViews>
@@ -908,7 +908,7 @@
     <t>The docks, offices and fishing piers of Fergal's Finest, one of the premier fisheries on the island.</t>
   </si>
   <si>
-    <t>Fountains of the Six Shrines</t>
+    <t>https://new.merisyl.com/gazette/chayle/aodar/aodar-free-city-map/?lng=-3004&amp;lat=-2876&amp;zoom=8||Fountain of the Six Shrines</t>
   </si>
 </sst>
 </file>
@@ -1333,7 +1333,7 @@
   <dimension ref="A1:D166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,7 +1359,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2745,7 +2745,7 @@
       </c>
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>

</xml_diff>